<commit_message>
changes in Upload Excel Template
</commit_message>
<xml_diff>
--- a/ExcelTemplates/ProviderDataUploadTemplate.xlsx
+++ b/ExcelTemplates/ProviderDataUploadTemplate.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irfan.Ahmad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkingProject\Source\Repos\VendorAPIWeb\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VendorList" sheetId="1" r:id="rId1"/>
+    <sheet name="IssueList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -50,46 +51,222 @@
     <t>Update</t>
   </si>
   <si>
-    <t>Henry Schine</t>
-  </si>
-  <si>
     <t>Martha</t>
   </si>
   <si>
     <t>On Boarding</t>
   </si>
   <si>
-    <t>Integration</t>
-  </si>
-  <si>
     <t>IFM</t>
   </si>
   <si>
-    <t>Integration is ongoing</t>
-  </si>
-  <si>
-    <t>IssueItem</t>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>VendorCode</t>
+  </si>
+  <si>
+    <t>Henry Schein</t>
+  </si>
+  <si>
+    <t>Waived for SBI</t>
+  </si>
+  <si>
+    <t>Test work orders and script samples provided 2/23/20. Henry Schein advised that they are targeting some UAT testing the week of 2/24.</t>
+  </si>
+  <si>
+    <t>FMO</t>
+  </si>
+  <si>
+    <t>HS001</t>
+  </si>
+  <si>
+    <t>Brightview</t>
+  </si>
+  <si>
+    <t>BV001</t>
+  </si>
+  <si>
+    <t>Staging Whitelisted</t>
+  </si>
+  <si>
+    <t>12,000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White listing and tokens issued 1/6/20. API L1 Help Desk providing support.   Call scheduled for 2/25/20 to discuss API use with Home Depot.              </t>
+  </si>
+  <si>
+    <t>Paintzen</t>
+  </si>
+  <si>
+    <t>PT001</t>
+  </si>
+  <si>
+    <t>QA Certification</t>
+  </si>
+  <si>
+    <t>Provider passed QA prep, QA certification call scheduled for 2/27/20.</t>
+  </si>
+  <si>
+    <t>PC Maintenance/Smartsheet</t>
+  </si>
+  <si>
+    <t>PC001</t>
+  </si>
+  <si>
+    <t>Waive Cost for HD</t>
+  </si>
+  <si>
+    <t>Provider attempted QA certification 2/19/20 but API call resulted in duplicate work orders in vendor Smartsheet. QA Certification re-scheduled for 2/28/20.</t>
+  </si>
+  <si>
+    <t>PTR Baler</t>
+  </si>
+  <si>
+    <t>PB001</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>02/27/2020</t>
+  </si>
+  <si>
+    <t>02/28/2020</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>FMO/IFM</t>
+  </si>
+  <si>
+    <t>Provider has been white listed and testing token provided Jan 24th. Help desk has been providing test work orders.</t>
+  </si>
+  <si>
+    <t>Academy Fire</t>
+  </si>
+  <si>
+    <t>AF001</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Attended kick off meeting Jan 21st. Links to API vendor support web page and connector manual provided. Provider declined STPL developer option.</t>
+  </si>
+  <si>
+    <t>MaintenX</t>
+  </si>
+  <si>
+    <t>MX001</t>
+  </si>
+  <si>
+    <t>Waived</t>
+  </si>
+  <si>
+    <t>Agreements signed 1/23. Fees waived per Josh. QA testing requirements provided. Maintenx sent response to follow up email stating that they are still in planning stages and not yet ready for testing.</t>
+  </si>
+  <si>
+    <t>Century Fire protection</t>
+  </si>
+  <si>
+    <t>CP001</t>
+  </si>
+  <si>
+    <t>Agreements sent to provide Jan 29th. Provider also sent link to register for weekly provider kick off call along with presentation deck.</t>
+  </si>
+  <si>
+    <t>Nixon</t>
+  </si>
+  <si>
+    <t>NX001</t>
+  </si>
+  <si>
+    <t>Nixon attended kick off call 11/14/19 and is now adding Home Depot, Office Depot and Davita.</t>
+  </si>
+  <si>
+    <t>Phoenix Technologies</t>
+  </si>
+  <si>
+    <t>PX001</t>
+  </si>
+  <si>
+    <t>2/10 provider will be testing with Office Depot. They have not specifically asked for any test work orders at this time.</t>
+  </si>
+  <si>
+    <t>Telgian</t>
+  </si>
+  <si>
+    <t>TG001</t>
+  </si>
+  <si>
+    <t>Ph 2 - In process</t>
+  </si>
+  <si>
+    <t>Testing Quotes</t>
+  </si>
+  <si>
+    <t>The provider went live in January with phase 1.They are currently adding the quote feature to their API. A bug fix is being released in production on 2/26 so that they can roll their quote API into production.</t>
+  </si>
+  <si>
+    <t>Park Construction</t>
+  </si>
+  <si>
+    <t>PK001</t>
+  </si>
+  <si>
+    <t>White Listing</t>
+  </si>
+  <si>
+    <t>2/25 in process to white list and issue a token for Home Depot and Davita.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NA001</t>
+  </si>
+  <si>
+    <t>FMO UPS</t>
+  </si>
+  <si>
+    <t>High priority provider, pending information on move of all UPS vendors to SI7</t>
+  </si>
+  <si>
+    <t>PC002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High priority provider, </t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
   <si>
     <t>Owner</t>
   </si>
   <si>
-    <t>IssueNo</t>
-  </si>
-  <si>
-    <t>AC repair</t>
-  </si>
-  <si>
-    <t>Robert Sandford</t>
+    <t>Quote bug fix required in FmPilot- QA testing being completed and added to branch</t>
+  </si>
+  <si>
+    <t>Lordell</t>
+  </si>
+  <si>
+    <t>Need confirmation that provder is approved to do business with Davita</t>
+  </si>
+  <si>
+    <t>Josh Casto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="0.00;[Red]0.00"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -114,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,47 +314,33 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,162 +621,596 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="9"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="182.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="10" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
-        <v>43920</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8">
-        <v>5000</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2">
-        <v>123</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="G6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
-      <formula1>"IFM,FMO"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+      <formula1>"FMO,IFM,FMO/IFM,FMO UPS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
-      <formula1>"Integration,On boarding"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+      <formula1>"Testing,QA Certification,Planning,Testing Quotes,White Listing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
-      <formula1>"Staging Whitelisted,On boarding"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>"On Boarding,Staging Whitelisted,Live"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>